<commit_message>
Update course codes spreadsheet
</commit_message>
<xml_diff>
--- a/public/Sheets/coures-codes.xlsx
+++ b/public/Sheets/coures-codes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WebDev\Learnings\drag and drop 2 working\currently working\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WebDev\github_repo\acad_council\Academic-Council\public\Sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{887936B4-BD7A-4437-9A4C-C056776FDCDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38DC0DAC-76C8-42C9-9A3C-83BE1924A0BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23016" windowHeight="12240" tabRatio="621" activeTab="3" xr2:uid="{4F99AE54-91E4-4B1C-BDED-A7482F8C8E09}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="621" activeTab="4" xr2:uid="{4F99AE54-91E4-4B1C-BDED-A7482F8C8E09}"/>
   </bookViews>
   <sheets>
     <sheet name="year 2019" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1335" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1335" uniqueCount="172">
   <si>
     <t>Branch</t>
   </si>
@@ -357,283 +357,205 @@
     <t>AI</t>
   </si>
   <si>
-    <t>FP:100</t>
-  </si>
-  <si>
-    <t>HS:191</t>
-  </si>
-  <si>
-    <t>HS:221</t>
-  </si>
-  <si>
-    <t>MA:103</t>
-  </si>
-  <si>
-    <t>ES:101</t>
-  </si>
-  <si>
-    <t>ES:112</t>
-  </si>
-  <si>
-    <t>ES:117</t>
-  </si>
-  <si>
-    <t>ES:118</t>
-  </si>
-  <si>
-    <t>PE:101</t>
-  </si>
-  <si>
-    <t>GE:101</t>
-  </si>
-  <si>
-    <t>HS:192</t>
-  </si>
-  <si>
-    <t>MA:104</t>
-  </si>
-  <si>
-    <t>BS:192</t>
-  </si>
-  <si>
-    <t>ES:113</t>
-  </si>
-  <si>
-    <t>ES:114</t>
-  </si>
-  <si>
-    <t>ES:115</t>
-  </si>
-  <si>
-    <t>ES:116</t>
-  </si>
-  <si>
-    <t>PE:102</t>
-  </si>
-  <si>
-    <t>GE:201</t>
-  </si>
-  <si>
-    <t>HS:151</t>
-  </si>
-  <si>
-    <t>MA:203</t>
-  </si>
-  <si>
-    <t>BS:XXX</t>
-  </si>
-  <si>
-    <t>ES:243</t>
-  </si>
-  <si>
-    <t>ES:242</t>
-  </si>
-  <si>
-    <t>ES:244</t>
-  </si>
-  <si>
-    <t>PE:103</t>
-  </si>
-  <si>
-    <t>HS:201</t>
-  </si>
-  <si>
-    <t>MA:XXX</t>
-  </si>
-  <si>
-    <t>ES:204</t>
-  </si>
-  <si>
-    <t>ES:245</t>
-  </si>
-  <si>
-    <t>CS:201</t>
-  </si>
-  <si>
-    <t>CS:303</t>
-  </si>
-  <si>
-    <t>PE:104</t>
-  </si>
-  <si>
-    <t>HS:XXX</t>
-  </si>
-  <si>
-    <t>ES:XXX</t>
-  </si>
-  <si>
-    <t>CS:329</t>
-  </si>
-  <si>
-    <t>ES:335</t>
-  </si>
-  <si>
-    <t>CS:328</t>
-  </si>
-  <si>
-    <t>ES:211</t>
-  </si>
-  <si>
-    <t>CL:201</t>
-  </si>
-  <si>
-    <t>CL:202</t>
-  </si>
-  <si>
-    <t>CL:203</t>
-  </si>
-  <si>
-    <t>CL:204</t>
-  </si>
-  <si>
-    <t>CL:205</t>
-  </si>
-  <si>
-    <t>CL:313</t>
-  </si>
-  <si>
-    <t>CL:314</t>
-  </si>
-  <si>
-    <t>CL:315</t>
-  </si>
-  <si>
-    <t>CL:326</t>
-  </si>
-  <si>
-    <t>CL:316</t>
-  </si>
-  <si>
-    <t>CL:317</t>
-  </si>
-  <si>
-    <t>CL:325</t>
-  </si>
-  <si>
-    <t>CL:327</t>
-  </si>
-  <si>
-    <t>ES:221</t>
-  </si>
-  <si>
-    <t>CE:201</t>
-  </si>
-  <si>
-    <t>CE:203</t>
-  </si>
-  <si>
-    <t>ES:212</t>
-  </si>
-  <si>
-    <t>CE:202</t>
-  </si>
-  <si>
-    <t>CE:302</t>
-  </si>
-  <si>
-    <t>CE:XXX</t>
-  </si>
-  <si>
-    <t>CE:301</t>
-  </si>
-  <si>
-    <t>CE:310</t>
-  </si>
-  <si>
-    <t>CE:312</t>
-  </si>
-  <si>
-    <t>CE:311</t>
-  </si>
-  <si>
-    <t>CE:403</t>
-  </si>
-  <si>
-    <t>ES:214</t>
-  </si>
-  <si>
-    <t>XX:XXX</t>
-  </si>
-  <si>
     <t>PH 201</t>
   </si>
   <si>
-    <t>EE:221</t>
-  </si>
-  <si>
-    <t>EE:223</t>
-  </si>
-  <si>
-    <t>EE:224</t>
-  </si>
-  <si>
-    <t>EE:312</t>
-  </si>
-  <si>
-    <t>EE:322</t>
-  </si>
-  <si>
-    <t>EE:323</t>
-  </si>
-  <si>
-    <t>EE:333</t>
-  </si>
-  <si>
-    <t>EE:313</t>
-  </si>
-  <si>
-    <t>MSE:202</t>
-  </si>
-  <si>
-    <t>MSE:204</t>
-  </si>
-  <si>
-    <t>MSE:207</t>
-  </si>
-  <si>
-    <t>MSE:203</t>
-  </si>
-  <si>
-    <t>MSE:205</t>
-  </si>
-  <si>
-    <t>MSE:206</t>
-  </si>
-  <si>
-    <t>MSE:210</t>
-  </si>
-  <si>
-    <t>MSE:307</t>
-  </si>
-  <si>
-    <t>MSE:313</t>
-  </si>
-  <si>
-    <t>MSE:302</t>
-  </si>
-  <si>
-    <t>MSE:312</t>
-  </si>
-  <si>
-    <t>ME:206</t>
-  </si>
-  <si>
-    <t>ME:207</t>
-  </si>
-  <si>
-    <t>ME:208</t>
-  </si>
-  <si>
-    <t>ME:209</t>
-  </si>
-  <si>
-    <t>ME:333</t>
-  </si>
-  <si>
-    <t>ME:334</t>
-  </si>
-  <si>
-    <t>ME:335</t>
+    <t>HS 191</t>
+  </si>
+  <si>
+    <t>MA 103</t>
+  </si>
+  <si>
+    <t>ES 117</t>
+  </si>
+  <si>
+    <t>ES 118</t>
+  </si>
+  <si>
+    <t>GE 101</t>
+  </si>
+  <si>
+    <t>HS 192</t>
+  </si>
+  <si>
+    <t>MA 104</t>
+  </si>
+  <si>
+    <t>BS 192</t>
+  </si>
+  <si>
+    <t>ES 113</t>
+  </si>
+  <si>
+    <t>ES 114</t>
+  </si>
+  <si>
+    <t>ES 115</t>
+  </si>
+  <si>
+    <t>ES 116</t>
+  </si>
+  <si>
+    <t>GE 201</t>
+  </si>
+  <si>
+    <t>MA 203</t>
+  </si>
+  <si>
+    <t>BS XXX</t>
+  </si>
+  <si>
+    <t>ES 243</t>
+  </si>
+  <si>
+    <t>MA XXX</t>
+  </si>
+  <si>
+    <t>CL 202</t>
+  </si>
+  <si>
+    <t>CL 203</t>
+  </si>
+  <si>
+    <t>CL 204</t>
+  </si>
+  <si>
+    <t>CL 205</t>
+  </si>
+  <si>
+    <t>HS XXX</t>
+  </si>
+  <si>
+    <t>CL 313</t>
+  </si>
+  <si>
+    <t>CL 314</t>
+  </si>
+  <si>
+    <t>CL 315</t>
+  </si>
+  <si>
+    <t>CL 326</t>
+  </si>
+  <si>
+    <t>CL 316</t>
+  </si>
+  <si>
+    <t>CL 317</t>
+  </si>
+  <si>
+    <t>CL 325</t>
+  </si>
+  <si>
+    <t>CL 327</t>
+  </si>
+  <si>
+    <t>CE 203</t>
+  </si>
+  <si>
+    <t>CE XXX</t>
+  </si>
+  <si>
+    <t>CE 310</t>
+  </si>
+  <si>
+    <t>CE 312</t>
+  </si>
+  <si>
+    <t>CE 311</t>
+  </si>
+  <si>
+    <t>ES 204</t>
+  </si>
+  <si>
+    <t>CS 201</t>
+  </si>
+  <si>
+    <t>XX XXX</t>
+  </si>
+  <si>
+    <t>CS 329</t>
+  </si>
+  <si>
+    <t>ES 244</t>
+  </si>
+  <si>
+    <t>EE 223</t>
+  </si>
+  <si>
+    <t>EE 224</t>
+  </si>
+  <si>
+    <t>ES 245</t>
+  </si>
+  <si>
+    <t>EE 312</t>
+  </si>
+  <si>
+    <t>EE 322</t>
+  </si>
+  <si>
+    <t>EE 323</t>
+  </si>
+  <si>
+    <t>EE 313</t>
+  </si>
+  <si>
+    <t>MSE 202</t>
+  </si>
+  <si>
+    <t>MSE 204</t>
+  </si>
+  <si>
+    <t>MSE 207</t>
+  </si>
+  <si>
+    <t>MSE 203</t>
+  </si>
+  <si>
+    <t>MSE 205</t>
+  </si>
+  <si>
+    <t>MSE 206</t>
+  </si>
+  <si>
+    <t>MSE 210</t>
+  </si>
+  <si>
+    <t>MSE 313</t>
+  </si>
+  <si>
+    <t>MSE 312</t>
+  </si>
+  <si>
+    <t>ME 206</t>
+  </si>
+  <si>
+    <t>ME 207</t>
+  </si>
+  <si>
+    <t>ME 208</t>
+  </si>
+  <si>
+    <t>ME 209</t>
+  </si>
+  <si>
+    <t>ME 333</t>
+  </si>
+  <si>
+    <t>ME 334</t>
+  </si>
+  <si>
+    <t>ME 335</t>
+  </si>
+  <si>
+    <t>CS 303</t>
+  </si>
+  <si>
+    <t>ES XXX</t>
+  </si>
+  <si>
+    <t>ES 335</t>
   </si>
 </sst>
 </file>
@@ -1047,8 +969,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0DEEA36-C6B7-4D02-8228-F75E679A42F6}">
   <dimension ref="A1:AR7"/>
   <sheetViews>
-    <sheetView topLeftCell="Y1" zoomScale="105" workbookViewId="0">
-      <selection activeCell="Z23" sqref="Z23"/>
+    <sheetView zoomScale="105" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1837,6 +1759,7 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1845,7 +1768,7 @@
   <dimension ref="A1:AR7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2633,6 +2556,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2641,7 +2565,7 @@
   <dimension ref="A1:AR7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3429,6 +3353,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3436,8 +3361,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51F375D9-59A9-4813-B46F-2527C5B30635}">
   <dimension ref="A1:AT7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3455,139 +3380,139 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>105</v>
+        <v>9</v>
       </c>
       <c r="C2" t="s">
         <v>106</v>
       </c>
       <c r="D2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" t="s">
         <v>107</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" t="s">
+        <v>42</v>
+      </c>
+      <c r="H2" t="s">
         <v>108</v>
       </c>
-      <c r="F2" t="s">
+      <c r="I2" t="s">
         <v>109</v>
       </c>
-      <c r="G2" t="s">
+      <c r="J2" t="s">
+        <v>13</v>
+      </c>
+      <c r="K2" t="s">
         <v>110</v>
       </c>
-      <c r="H2" t="s">
+      <c r="L2" t="s">
         <v>111</v>
       </c>
-      <c r="I2" t="s">
+      <c r="M2" t="s">
         <v>112</v>
       </c>
-      <c r="J2" t="s">
+      <c r="N2" t="s">
         <v>113</v>
       </c>
-      <c r="K2" t="s">
+      <c r="O2" t="s">
         <v>114</v>
       </c>
-      <c r="L2" t="s">
+      <c r="P2" t="s">
         <v>115</v>
       </c>
-      <c r="M2" t="s">
+      <c r="Q2" t="s">
         <v>116</v>
       </c>
-      <c r="N2" t="s">
+      <c r="R2" t="s">
         <v>117</v>
       </c>
-      <c r="O2" t="s">
+      <c r="S2" t="s">
+        <v>8</v>
+      </c>
+      <c r="T2" t="s">
         <v>118</v>
       </c>
-      <c r="P2" t="s">
+      <c r="U2" t="s">
+        <v>14</v>
+      </c>
+      <c r="V2" t="s">
         <v>119</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="W2" t="s">
         <v>120</v>
       </c>
-      <c r="R2" t="s">
+      <c r="X2" t="s">
         <v>121</v>
       </c>
-      <c r="S2" t="s">
+      <c r="Y2" t="s">
+        <v>47</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>48</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>29</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>30</v>
+      </c>
+      <c r="AC2" t="s">
         <v>122</v>
       </c>
-      <c r="T2" t="s">
+      <c r="AD2" t="s">
+        <v>120</v>
+      </c>
+      <c r="AE2" t="s">
         <v>123</v>
       </c>
-      <c r="U2" t="s">
+      <c r="AF2" t="s">
         <v>124</v>
       </c>
-      <c r="V2" t="s">
+      <c r="AG2" t="s">
         <v>125</v>
       </c>
-      <c r="W2" t="s">
+      <c r="AH2" t="s">
         <v>126</v>
       </c>
-      <c r="X2" t="s">
+      <c r="AI2" t="s">
+        <v>35</v>
+      </c>
+      <c r="AJ2" t="s">
         <v>127</v>
       </c>
-      <c r="Y2" t="s">
-        <v>143</v>
-      </c>
-      <c r="Z2" t="s">
-        <v>144</v>
-      </c>
-      <c r="AA2" t="s">
+      <c r="AK2" t="s">
+        <v>128</v>
+      </c>
+      <c r="AL2" t="s">
+        <v>129</v>
+      </c>
+      <c r="AM2" t="s">
         <v>130</v>
       </c>
-      <c r="AB2" t="s">
+      <c r="AN2" t="s">
         <v>131</v>
       </c>
-      <c r="AC2" t="s">
+      <c r="AO2" t="s">
+        <v>127</v>
+      </c>
+      <c r="AP2" t="s">
         <v>132</v>
       </c>
-      <c r="AD2" t="s">
-        <v>126</v>
-      </c>
-      <c r="AE2" t="s">
-        <v>145</v>
-      </c>
-      <c r="AF2" t="s">
-        <v>146</v>
-      </c>
-      <c r="AG2" t="s">
-        <v>147</v>
-      </c>
-      <c r="AH2" t="s">
-        <v>148</v>
-      </c>
-      <c r="AI2" t="s">
-        <v>137</v>
-      </c>
-      <c r="AJ2" t="s">
-        <v>138</v>
-      </c>
-      <c r="AK2" t="s">
-        <v>149</v>
-      </c>
-      <c r="AL2" t="s">
-        <v>150</v>
-      </c>
-      <c r="AM2" t="s">
-        <v>151</v>
-      </c>
-      <c r="AN2" t="s">
-        <v>152</v>
-      </c>
-      <c r="AO2" t="s">
-        <v>138</v>
-      </c>
-      <c r="AP2" t="s">
-        <v>153</v>
-      </c>
       <c r="AQ2" t="s">
-        <v>154</v>
+        <v>133</v>
       </c>
       <c r="AR2" t="s">
-        <v>155</v>
+        <v>134</v>
       </c>
       <c r="AS2" t="s">
-        <v>156</v>
+        <v>135</v>
       </c>
       <c r="AT2" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
     </row>
     <row r="3" spans="1:46" x14ac:dyDescent="0.3">
@@ -3595,139 +3520,139 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>105</v>
+        <v>9</v>
       </c>
       <c r="C3" t="s">
         <v>106</v>
       </c>
       <c r="D3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" t="s">
         <v>107</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" t="s">
+        <v>42</v>
+      </c>
+      <c r="H3" t="s">
         <v>108</v>
       </c>
-      <c r="F3" t="s">
+      <c r="I3" t="s">
         <v>109</v>
       </c>
-      <c r="G3" t="s">
+      <c r="J3" t="s">
+        <v>13</v>
+      </c>
+      <c r="K3" t="s">
         <v>110</v>
       </c>
-      <c r="H3" t="s">
+      <c r="L3" t="s">
         <v>111</v>
       </c>
-      <c r="I3" t="s">
+      <c r="M3" t="s">
         <v>112</v>
       </c>
-      <c r="J3" t="s">
+      <c r="N3" t="s">
         <v>113</v>
       </c>
-      <c r="K3" t="s">
+      <c r="O3" t="s">
         <v>114</v>
       </c>
-      <c r="L3" t="s">
+      <c r="P3" t="s">
         <v>115</v>
       </c>
-      <c r="M3" t="s">
+      <c r="Q3" t="s">
         <v>116</v>
       </c>
-      <c r="N3" t="s">
+      <c r="R3" t="s">
         <v>117</v>
       </c>
-      <c r="O3" t="s">
+      <c r="S3" t="s">
+        <v>8</v>
+      </c>
+      <c r="T3" t="s">
         <v>118</v>
       </c>
-      <c r="P3" t="s">
+      <c r="U3" t="s">
+        <v>14</v>
+      </c>
+      <c r="V3" t="s">
         <v>119</v>
       </c>
-      <c r="Q3" t="s">
+      <c r="W3" t="s">
         <v>120</v>
       </c>
-      <c r="R3" t="s">
+      <c r="X3" t="s">
         <v>121</v>
       </c>
-      <c r="S3" t="s">
+      <c r="Y3" t="s">
+        <v>45</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>136</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>29</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>30</v>
+      </c>
+      <c r="AD3" t="s">
         <v>122</v>
       </c>
-      <c r="T3" t="s">
-        <v>123</v>
-      </c>
-      <c r="U3" t="s">
-        <v>124</v>
-      </c>
-      <c r="V3" t="s">
-        <v>125</v>
-      </c>
-      <c r="W3" t="s">
-        <v>126</v>
-      </c>
-      <c r="X3" t="s">
+      <c r="AE3" t="s">
+        <v>120</v>
+      </c>
+      <c r="AF3" t="s">
+        <v>44</v>
+      </c>
+      <c r="AG3" t="s">
+        <v>51</v>
+      </c>
+      <c r="AH3" t="s">
+        <v>63</v>
+      </c>
+      <c r="AI3" t="s">
+        <v>137</v>
+      </c>
+      <c r="AJ3" t="s">
+        <v>35</v>
+      </c>
+      <c r="AK3" t="s">
         <v>127</v>
       </c>
-      <c r="Y3" t="s">
-        <v>157</v>
-      </c>
-      <c r="Z3" t="s">
-        <v>158</v>
-      </c>
-      <c r="AA3" t="s">
-        <v>159</v>
-      </c>
-      <c r="AB3" t="s">
-        <v>130</v>
-      </c>
-      <c r="AC3" t="s">
-        <v>131</v>
-      </c>
-      <c r="AD3" t="s">
-        <v>132</v>
-      </c>
-      <c r="AE3" t="s">
-        <v>126</v>
-      </c>
-      <c r="AF3" t="s">
-        <v>160</v>
-      </c>
-      <c r="AG3" t="s">
-        <v>161</v>
-      </c>
-      <c r="AH3" t="s">
-        <v>162</v>
-      </c>
-      <c r="AI3" t="s">
-        <v>163</v>
-      </c>
-      <c r="AJ3" t="s">
+      <c r="AL3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AM3" t="s">
+        <v>138</v>
+      </c>
+      <c r="AN3" t="s">
+        <v>139</v>
+      </c>
+      <c r="AO3" t="s">
+        <v>127</v>
+      </c>
+      <c r="AP3" t="s">
+        <v>140</v>
+      </c>
+      <c r="AQ3" t="s">
         <v>137</v>
       </c>
-      <c r="AK3" t="s">
-        <v>138</v>
-      </c>
-      <c r="AL3" t="s">
-        <v>164</v>
-      </c>
-      <c r="AM3" t="s">
-        <v>165</v>
-      </c>
-      <c r="AN3" t="s">
-        <v>166</v>
-      </c>
-      <c r="AO3" t="s">
-        <v>138</v>
-      </c>
-      <c r="AP3" t="s">
-        <v>167</v>
-      </c>
-      <c r="AQ3" t="s">
-        <v>163</v>
-      </c>
       <c r="AR3" t="s">
-        <v>163</v>
+        <v>137</v>
       </c>
       <c r="AS3" t="s">
-        <v>168</v>
+        <v>70</v>
       </c>
       <c r="AT3" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
     </row>
     <row r="4" spans="1:46" x14ac:dyDescent="0.3">
@@ -3735,130 +3660,130 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>105</v>
+        <v>9</v>
       </c>
       <c r="C4" t="s">
         <v>106</v>
       </c>
       <c r="D4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" t="s">
         <v>107</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" t="s">
+        <v>42</v>
+      </c>
+      <c r="H4" t="s">
         <v>108</v>
       </c>
-      <c r="F4" t="s">
+      <c r="I4" t="s">
         <v>109</v>
       </c>
-      <c r="G4" t="s">
+      <c r="J4" t="s">
+        <v>13</v>
+      </c>
+      <c r="K4" t="s">
         <v>110</v>
       </c>
-      <c r="H4" t="s">
+      <c r="L4" t="s">
         <v>111</v>
       </c>
-      <c r="I4" t="s">
+      <c r="M4" t="s">
         <v>112</v>
       </c>
-      <c r="J4" t="s">
+      <c r="N4" t="s">
         <v>113</v>
       </c>
-      <c r="K4" t="s">
+      <c r="O4" t="s">
         <v>114</v>
       </c>
-      <c r="L4" t="s">
+      <c r="P4" t="s">
         <v>115</v>
       </c>
-      <c r="M4" t="s">
+      <c r="Q4" t="s">
         <v>116</v>
       </c>
-      <c r="N4" t="s">
+      <c r="R4" t="s">
         <v>117</v>
       </c>
-      <c r="O4" t="s">
+      <c r="S4" t="s">
+        <v>8</v>
+      </c>
+      <c r="T4" t="s">
         <v>118</v>
       </c>
-      <c r="P4" t="s">
+      <c r="U4" t="s">
+        <v>14</v>
+      </c>
+      <c r="V4" t="s">
         <v>119</v>
       </c>
-      <c r="Q4" t="s">
+      <c r="W4" t="s">
         <v>120</v>
       </c>
-      <c r="R4" t="s">
+      <c r="X4" t="s">
         <v>121</v>
       </c>
-      <c r="S4" t="s">
+      <c r="Y4" t="s">
+        <v>33</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>26</v>
+      </c>
+      <c r="AA4" t="s">
+        <v>29</v>
+      </c>
+      <c r="AB4" t="s">
+        <v>30</v>
+      </c>
+      <c r="AC4" t="s">
         <v>122</v>
       </c>
-      <c r="T4" t="s">
-        <v>123</v>
-      </c>
-      <c r="U4" t="s">
-        <v>124</v>
-      </c>
-      <c r="V4" t="s">
-        <v>125</v>
-      </c>
-      <c r="W4" t="s">
-        <v>126</v>
-      </c>
-      <c r="X4" t="s">
+      <c r="AD4" t="s">
+        <v>120</v>
+      </c>
+      <c r="AE4" t="s">
+        <v>141</v>
+      </c>
+      <c r="AF4" t="s">
+        <v>142</v>
+      </c>
+      <c r="AG4" t="s">
+        <v>143</v>
+      </c>
+      <c r="AH4" t="s">
+        <v>143</v>
+      </c>
+      <c r="AI4" t="s">
+        <v>35</v>
+      </c>
+      <c r="AJ4" t="s">
         <v>127</v>
       </c>
-      <c r="Y4" t="s">
-        <v>169</v>
-      </c>
-      <c r="Z4" t="s">
-        <v>128</v>
-      </c>
-      <c r="AA4" t="s">
-        <v>130</v>
-      </c>
-      <c r="AB4" t="s">
-        <v>131</v>
-      </c>
-      <c r="AC4" t="s">
-        <v>132</v>
-      </c>
-      <c r="AD4" t="s">
-        <v>126</v>
-      </c>
-      <c r="AE4" t="s">
-        <v>133</v>
-      </c>
-      <c r="AF4" t="s">
-        <v>135</v>
-      </c>
-      <c r="AG4" t="s">
-        <v>170</v>
-      </c>
-      <c r="AH4" t="s">
-        <v>170</v>
-      </c>
-      <c r="AI4" t="s">
-        <v>137</v>
-      </c>
-      <c r="AJ4" t="s">
-        <v>138</v>
-      </c>
       <c r="AK4" t="s">
-        <v>170</v>
+        <v>143</v>
       </c>
       <c r="AL4" t="s">
-        <v>170</v>
+        <v>143</v>
       </c>
       <c r="AM4" t="s">
-        <v>170</v>
+        <v>143</v>
       </c>
       <c r="AN4" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="AO4" t="s">
-        <v>138</v>
+        <v>127</v>
       </c>
       <c r="AP4" t="s">
-        <v>138</v>
+        <v>127</v>
       </c>
       <c r="AQ4" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
     </row>
     <row r="5" spans="1:46" x14ac:dyDescent="0.3">
@@ -3866,130 +3791,130 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>105</v>
+        <v>9</v>
       </c>
       <c r="C5" t="s">
         <v>106</v>
       </c>
       <c r="D5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" t="s">
         <v>107</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" t="s">
+        <v>42</v>
+      </c>
+      <c r="H5" t="s">
         <v>108</v>
       </c>
-      <c r="F5" t="s">
+      <c r="I5" t="s">
         <v>109</v>
       </c>
-      <c r="G5" t="s">
+      <c r="J5" t="s">
+        <v>13</v>
+      </c>
+      <c r="K5" t="s">
         <v>110</v>
       </c>
-      <c r="H5" t="s">
+      <c r="L5" t="s">
         <v>111</v>
       </c>
-      <c r="I5" t="s">
+      <c r="M5" t="s">
         <v>112</v>
       </c>
-      <c r="J5" t="s">
+      <c r="N5" t="s">
         <v>113</v>
       </c>
-      <c r="K5" t="s">
+      <c r="O5" t="s">
         <v>114</v>
       </c>
-      <c r="L5" t="s">
+      <c r="P5" t="s">
         <v>115</v>
       </c>
-      <c r="M5" t="s">
+      <c r="Q5" t="s">
         <v>116</v>
       </c>
-      <c r="N5" t="s">
+      <c r="R5" t="s">
         <v>117</v>
       </c>
-      <c r="O5" t="s">
+      <c r="S5" t="s">
+        <v>8</v>
+      </c>
+      <c r="T5" t="s">
         <v>118</v>
       </c>
-      <c r="P5" t="s">
+      <c r="U5" t="s">
+        <v>14</v>
+      </c>
+      <c r="V5" t="s">
         <v>119</v>
       </c>
-      <c r="Q5" t="s">
+      <c r="W5" t="s">
+        <v>105</v>
+      </c>
+      <c r="X5" t="s">
+        <v>121</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>145</v>
+      </c>
+      <c r="Z5" t="s">
+        <v>73</v>
+      </c>
+      <c r="AA5" t="s">
+        <v>146</v>
+      </c>
+      <c r="AB5" t="s">
+        <v>29</v>
+      </c>
+      <c r="AC5" t="s">
+        <v>30</v>
+      </c>
+      <c r="AD5" t="s">
+        <v>122</v>
+      </c>
+      <c r="AE5" t="s">
         <v>120</v>
       </c>
-      <c r="R5" t="s">
-        <v>121</v>
-      </c>
-      <c r="S5" t="s">
-        <v>122</v>
-      </c>
-      <c r="T5" t="s">
-        <v>123</v>
-      </c>
-      <c r="U5" t="s">
-        <v>124</v>
-      </c>
-      <c r="V5" t="s">
-        <v>125</v>
-      </c>
-      <c r="W5" t="s">
-        <v>171</v>
-      </c>
-      <c r="X5" t="s">
+      <c r="AF5" t="s">
+        <v>141</v>
+      </c>
+      <c r="AG5" t="s">
+        <v>147</v>
+      </c>
+      <c r="AH5" t="s">
+        <v>148</v>
+      </c>
+      <c r="AI5" t="s">
+        <v>35</v>
+      </c>
+      <c r="AJ5" t="s">
         <v>127</v>
       </c>
-      <c r="Y5" t="s">
-        <v>129</v>
-      </c>
-      <c r="Z5" t="s">
-        <v>172</v>
-      </c>
-      <c r="AA5" t="s">
-        <v>173</v>
-      </c>
-      <c r="AB5" t="s">
-        <v>130</v>
-      </c>
-      <c r="AC5" t="s">
-        <v>131</v>
-      </c>
-      <c r="AD5" t="s">
-        <v>132</v>
-      </c>
-      <c r="AE5" t="s">
-        <v>126</v>
-      </c>
-      <c r="AF5" t="s">
-        <v>133</v>
-      </c>
-      <c r="AG5" t="s">
-        <v>174</v>
-      </c>
-      <c r="AH5" t="s">
-        <v>134</v>
-      </c>
-      <c r="AI5" t="s">
-        <v>137</v>
-      </c>
-      <c r="AJ5" t="s">
-        <v>138</v>
-      </c>
       <c r="AK5" t="s">
-        <v>175</v>
+        <v>149</v>
       </c>
       <c r="AL5" t="s">
-        <v>176</v>
+        <v>150</v>
       </c>
       <c r="AM5" t="s">
-        <v>177</v>
+        <v>151</v>
       </c>
       <c r="AN5" t="s">
-        <v>178</v>
+        <v>83</v>
       </c>
       <c r="AO5" t="s">
-        <v>138</v>
+        <v>127</v>
       </c>
       <c r="AP5" t="s">
-        <v>179</v>
+        <v>152</v>
       </c>
       <c r="AQ5" s="1" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
     </row>
     <row r="6" spans="1:46" x14ac:dyDescent="0.3">
@@ -3997,130 +3922,130 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>105</v>
+        <v>9</v>
       </c>
       <c r="C6" t="s">
         <v>106</v>
       </c>
       <c r="D6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" t="s">
         <v>107</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6" t="s">
+        <v>42</v>
+      </c>
+      <c r="H6" t="s">
         <v>108</v>
       </c>
-      <c r="F6" t="s">
+      <c r="I6" t="s">
         <v>109</v>
       </c>
-      <c r="G6" t="s">
+      <c r="J6" t="s">
+        <v>13</v>
+      </c>
+      <c r="K6" t="s">
         <v>110</v>
       </c>
-      <c r="H6" t="s">
+      <c r="L6" t="s">
         <v>111</v>
       </c>
-      <c r="I6" t="s">
+      <c r="M6" t="s">
         <v>112</v>
       </c>
-      <c r="J6" t="s">
+      <c r="N6" t="s">
         <v>113</v>
       </c>
-      <c r="K6" t="s">
+      <c r="O6" t="s">
         <v>114</v>
       </c>
-      <c r="L6" t="s">
+      <c r="P6" t="s">
         <v>115</v>
       </c>
-      <c r="M6" t="s">
+      <c r="Q6" t="s">
         <v>116</v>
       </c>
-      <c r="N6" t="s">
+      <c r="R6" t="s">
         <v>117</v>
       </c>
-      <c r="O6" t="s">
+      <c r="S6" t="s">
+        <v>8</v>
+      </c>
+      <c r="T6" t="s">
         <v>118</v>
       </c>
-      <c r="P6" t="s">
+      <c r="U6" t="s">
+        <v>14</v>
+      </c>
+      <c r="V6" t="s">
         <v>119</v>
       </c>
-      <c r="Q6" t="s">
+      <c r="W6" t="s">
+        <v>121</v>
+      </c>
+      <c r="X6" t="s">
+        <v>153</v>
+      </c>
+      <c r="Y6" t="s">
+        <v>154</v>
+      </c>
+      <c r="Z6" t="s">
+        <v>155</v>
+      </c>
+      <c r="AA6" t="s">
+        <v>29</v>
+      </c>
+      <c r="AB6" t="s">
+        <v>30</v>
+      </c>
+      <c r="AC6" t="s">
+        <v>122</v>
+      </c>
+      <c r="AD6" t="s">
+        <v>156</v>
+      </c>
+      <c r="AE6" t="s">
+        <v>157</v>
+      </c>
+      <c r="AF6" t="s">
+        <v>158</v>
+      </c>
+      <c r="AG6" t="s">
+        <v>159</v>
+      </c>
+      <c r="AH6" t="s">
+        <v>35</v>
+      </c>
+      <c r="AI6" t="s">
+        <v>127</v>
+      </c>
+      <c r="AJ6" t="s">
         <v>120</v>
       </c>
-      <c r="R6" t="s">
-        <v>121</v>
-      </c>
-      <c r="S6" t="s">
-        <v>122</v>
-      </c>
-      <c r="T6" t="s">
-        <v>123</v>
-      </c>
-      <c r="U6" t="s">
-        <v>124</v>
-      </c>
-      <c r="V6" t="s">
-        <v>125</v>
-      </c>
-      <c r="W6" t="s">
+      <c r="AK6" t="s">
+        <v>100</v>
+      </c>
+      <c r="AL6" t="s">
+        <v>160</v>
+      </c>
+      <c r="AM6" t="s">
         <v>127</v>
       </c>
-      <c r="X6" t="s">
-        <v>180</v>
-      </c>
-      <c r="Y6" t="s">
-        <v>181</v>
-      </c>
-      <c r="Z6" t="s">
-        <v>182</v>
-      </c>
-      <c r="AA6" t="s">
-        <v>130</v>
-      </c>
-      <c r="AB6" t="s">
-        <v>131</v>
-      </c>
-      <c r="AC6" t="s">
-        <v>132</v>
-      </c>
-      <c r="AD6" t="s">
-        <v>183</v>
-      </c>
-      <c r="AE6" t="s">
-        <v>184</v>
-      </c>
-      <c r="AF6" t="s">
-        <v>185</v>
-      </c>
-      <c r="AG6" t="s">
-        <v>186</v>
-      </c>
-      <c r="AH6" t="s">
-        <v>137</v>
-      </c>
-      <c r="AI6" t="s">
-        <v>138</v>
-      </c>
-      <c r="AJ6" t="s">
-        <v>126</v>
-      </c>
-      <c r="AK6" t="s">
-        <v>187</v>
-      </c>
-      <c r="AL6" t="s">
-        <v>188</v>
-      </c>
-      <c r="AM6" t="s">
-        <v>138</v>
-      </c>
       <c r="AN6" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="AO6" t="s">
-        <v>189</v>
+        <v>102</v>
       </c>
       <c r="AP6" t="s">
-        <v>190</v>
+        <v>161</v>
       </c>
       <c r="AQ6" s="1" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
     </row>
     <row r="7" spans="1:46" x14ac:dyDescent="0.3">
@@ -4128,128 +4053,129 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>105</v>
+        <v>9</v>
       </c>
       <c r="C7" t="s">
         <v>106</v>
       </c>
       <c r="D7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" t="s">
         <v>107</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7" t="s">
+        <v>42</v>
+      </c>
+      <c r="H7" t="s">
         <v>108</v>
       </c>
-      <c r="F7" t="s">
+      <c r="I7" t="s">
         <v>109</v>
       </c>
-      <c r="G7" t="s">
+      <c r="J7" t="s">
+        <v>13</v>
+      </c>
+      <c r="K7" t="s">
         <v>110</v>
       </c>
-      <c r="H7" t="s">
+      <c r="L7" t="s">
         <v>111</v>
       </c>
-      <c r="I7" t="s">
+      <c r="M7" t="s">
         <v>112</v>
       </c>
-      <c r="J7" t="s">
+      <c r="N7" t="s">
         <v>113</v>
       </c>
-      <c r="K7" t="s">
+      <c r="O7" t="s">
         <v>114</v>
       </c>
-      <c r="L7" t="s">
+      <c r="P7" t="s">
         <v>115</v>
       </c>
-      <c r="M7" t="s">
+      <c r="Q7" t="s">
         <v>116</v>
       </c>
-      <c r="N7" t="s">
+      <c r="R7" t="s">
         <v>117</v>
       </c>
-      <c r="O7" t="s">
+      <c r="S7" t="s">
+        <v>8</v>
+      </c>
+      <c r="T7" t="s">
         <v>118</v>
       </c>
-      <c r="P7" t="s">
+      <c r="U7" t="s">
+        <v>14</v>
+      </c>
+      <c r="V7" t="s">
         <v>119</v>
       </c>
-      <c r="Q7" t="s">
+      <c r="W7" t="s">
         <v>120</v>
       </c>
-      <c r="R7" t="s">
+      <c r="X7" t="s">
         <v>121</v>
       </c>
-      <c r="S7" t="s">
+      <c r="Y7" t="s">
+        <v>162</v>
+      </c>
+      <c r="Z7" t="s">
+        <v>29</v>
+      </c>
+      <c r="AA7" t="s">
+        <v>30</v>
+      </c>
+      <c r="AB7" t="s">
         <v>122</v>
       </c>
-      <c r="T7" t="s">
-        <v>123</v>
-      </c>
-      <c r="U7" t="s">
-        <v>124</v>
-      </c>
-      <c r="V7" t="s">
-        <v>125</v>
-      </c>
-      <c r="W7" t="s">
-        <v>126</v>
-      </c>
-      <c r="X7" t="s">
+      <c r="AC7" t="s">
+        <v>120</v>
+      </c>
+      <c r="AD7" t="s">
+        <v>45</v>
+      </c>
+      <c r="AE7" t="s">
+        <v>163</v>
+      </c>
+      <c r="AF7" t="s">
+        <v>164</v>
+      </c>
+      <c r="AG7" t="s">
+        <v>165</v>
+      </c>
+      <c r="AH7" t="s">
+        <v>35</v>
+      </c>
+      <c r="AI7" t="s">
         <v>127</v>
       </c>
-      <c r="Y7" t="s">
-        <v>191</v>
-      </c>
-      <c r="Z7" t="s">
-        <v>130</v>
-      </c>
-      <c r="AA7" t="s">
-        <v>131</v>
-      </c>
-      <c r="AB7" t="s">
-        <v>132</v>
-      </c>
-      <c r="AC7" t="s">
-        <v>126</v>
-      </c>
-      <c r="AD7" t="s">
-        <v>157</v>
-      </c>
-      <c r="AE7" t="s">
-        <v>192</v>
-      </c>
-      <c r="AF7" t="s">
-        <v>193</v>
-      </c>
-      <c r="AG7" t="s">
-        <v>194</v>
-      </c>
-      <c r="AH7" t="s">
-        <v>137</v>
-      </c>
-      <c r="AI7" t="s">
-        <v>138</v>
-      </c>
       <c r="AJ7" t="s">
-        <v>134</v>
+        <v>148</v>
       </c>
       <c r="AK7" t="s">
-        <v>195</v>
+        <v>166</v>
       </c>
       <c r="AL7" t="s">
-        <v>196</v>
+        <v>167</v>
       </c>
       <c r="AM7" t="s">
-        <v>197</v>
+        <v>168</v>
       </c>
       <c r="AN7" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="AO7" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -4257,8 +4183,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C638EA0-D83C-444A-9E93-000193994880}">
   <dimension ref="A1:AT8"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="Q12" sqref="Q12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M17" sqref="M17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4276,127 +4202,127 @@
         <v>104</v>
       </c>
       <c r="B2" t="s">
-        <v>105</v>
+        <v>9</v>
       </c>
       <c r="C2" t="s">
         <v>106</v>
       </c>
       <c r="D2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" t="s">
         <v>107</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" t="s">
+        <v>42</v>
+      </c>
+      <c r="H2" t="s">
         <v>108</v>
       </c>
-      <c r="F2" t="s">
+      <c r="I2" t="s">
         <v>109</v>
       </c>
-      <c r="G2" t="s">
+      <c r="J2" t="s">
+        <v>13</v>
+      </c>
+      <c r="K2" t="s">
         <v>110</v>
       </c>
-      <c r="H2" t="s">
+      <c r="L2" t="s">
         <v>111</v>
       </c>
-      <c r="I2" t="s">
+      <c r="M2" t="s">
         <v>112</v>
       </c>
-      <c r="J2" t="s">
+      <c r="N2" t="s">
         <v>113</v>
       </c>
-      <c r="K2" t="s">
+      <c r="O2" t="s">
         <v>114</v>
       </c>
-      <c r="L2" t="s">
+      <c r="P2" t="s">
         <v>115</v>
       </c>
-      <c r="M2" t="s">
+      <c r="Q2" t="s">
         <v>116</v>
       </c>
-      <c r="N2" t="s">
+      <c r="R2" t="s">
         <v>117</v>
       </c>
-      <c r="O2" t="s">
+      <c r="S2" t="s">
+        <v>8</v>
+      </c>
+      <c r="T2" t="s">
         <v>118</v>
       </c>
-      <c r="P2" t="s">
+      <c r="U2" t="s">
+        <v>14</v>
+      </c>
+      <c r="V2" t="s">
         <v>119</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="W2" t="s">
         <v>120</v>
       </c>
-      <c r="R2" t="s">
+      <c r="X2" t="s">
         <v>121</v>
       </c>
-      <c r="S2" t="s">
+      <c r="Y2" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>145</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>29</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>30</v>
+      </c>
+      <c r="AC2" t="s">
         <v>122</v>
       </c>
-      <c r="T2" t="s">
-        <v>123</v>
-      </c>
-      <c r="U2" t="s">
-        <v>124</v>
-      </c>
-      <c r="V2" t="s">
-        <v>125</v>
-      </c>
-      <c r="W2" t="s">
-        <v>126</v>
-      </c>
-      <c r="X2" t="s">
+      <c r="AD2" t="s">
+        <v>120</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>141</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>148</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>142</v>
+      </c>
+      <c r="AH2" t="s">
+        <v>169</v>
+      </c>
+      <c r="AI2" t="s">
+        <v>35</v>
+      </c>
+      <c r="AJ2" t="s">
         <v>127</v>
       </c>
-      <c r="Y2" t="s">
-        <v>128</v>
-      </c>
-      <c r="Z2" t="s">
-        <v>129</v>
-      </c>
-      <c r="AA2" t="s">
-        <v>130</v>
-      </c>
-      <c r="AB2" t="s">
-        <v>131</v>
-      </c>
-      <c r="AC2" t="s">
-        <v>132</v>
-      </c>
-      <c r="AD2" t="s">
-        <v>126</v>
-      </c>
-      <c r="AE2" t="s">
-        <v>133</v>
-      </c>
-      <c r="AF2" t="s">
-        <v>134</v>
-      </c>
-      <c r="AG2" t="s">
-        <v>135</v>
-      </c>
-      <c r="AH2" t="s">
-        <v>136</v>
-      </c>
-      <c r="AI2" t="s">
-        <v>137</v>
-      </c>
-      <c r="AJ2" t="s">
-        <v>138</v>
-      </c>
       <c r="AK2" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="AL2" t="s">
-        <v>139</v>
+        <v>170</v>
       </c>
       <c r="AM2" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="AN2" t="s">
-        <v>138</v>
+        <v>127</v>
       </c>
       <c r="AO2" t="s">
-        <v>141</v>
+        <v>171</v>
       </c>
       <c r="AP2" t="s">
-        <v>142</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:46" x14ac:dyDescent="0.3">
@@ -4404,139 +4330,139 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>105</v>
+        <v>9</v>
       </c>
       <c r="C3" t="s">
         <v>106</v>
       </c>
       <c r="D3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" t="s">
         <v>107</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" t="s">
+        <v>42</v>
+      </c>
+      <c r="H3" t="s">
         <v>108</v>
       </c>
-      <c r="F3" t="s">
+      <c r="I3" t="s">
         <v>109</v>
       </c>
-      <c r="G3" t="s">
+      <c r="J3" t="s">
+        <v>13</v>
+      </c>
+      <c r="K3" t="s">
         <v>110</v>
       </c>
-      <c r="H3" t="s">
+      <c r="L3" t="s">
         <v>111</v>
       </c>
-      <c r="I3" t="s">
+      <c r="M3" t="s">
         <v>112</v>
       </c>
-      <c r="J3" t="s">
+      <c r="N3" t="s">
         <v>113</v>
       </c>
-      <c r="K3" t="s">
+      <c r="O3" t="s">
         <v>114</v>
       </c>
-      <c r="L3" t="s">
+      <c r="P3" t="s">
         <v>115</v>
       </c>
-      <c r="M3" t="s">
+      <c r="Q3" t="s">
         <v>116</v>
       </c>
-      <c r="N3" t="s">
+      <c r="R3" t="s">
         <v>117</v>
       </c>
-      <c r="O3" t="s">
+      <c r="S3" t="s">
+        <v>8</v>
+      </c>
+      <c r="T3" t="s">
         <v>118</v>
       </c>
-      <c r="P3" t="s">
+      <c r="U3" t="s">
+        <v>14</v>
+      </c>
+      <c r="V3" t="s">
         <v>119</v>
       </c>
-      <c r="Q3" t="s">
+      <c r="W3" t="s">
         <v>120</v>
       </c>
-      <c r="R3" t="s">
+      <c r="X3" t="s">
         <v>121</v>
       </c>
-      <c r="S3" t="s">
+      <c r="Y3" t="s">
+        <v>47</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>48</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>29</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>30</v>
+      </c>
+      <c r="AC3" t="s">
         <v>122</v>
       </c>
-      <c r="T3" t="s">
+      <c r="AD3" t="s">
+        <v>120</v>
+      </c>
+      <c r="AE3" t="s">
         <v>123</v>
       </c>
-      <c r="U3" t="s">
+      <c r="AF3" t="s">
         <v>124</v>
       </c>
-      <c r="V3" t="s">
+      <c r="AG3" t="s">
         <v>125</v>
       </c>
-      <c r="W3" t="s">
+      <c r="AH3" t="s">
         <v>126</v>
       </c>
-      <c r="X3" t="s">
+      <c r="AI3" t="s">
+        <v>35</v>
+      </c>
+      <c r="AJ3" t="s">
         <v>127</v>
       </c>
-      <c r="Y3" t="s">
-        <v>143</v>
-      </c>
-      <c r="Z3" t="s">
-        <v>144</v>
-      </c>
-      <c r="AA3" t="s">
+      <c r="AK3" t="s">
+        <v>128</v>
+      </c>
+      <c r="AL3" t="s">
+        <v>129</v>
+      </c>
+      <c r="AM3" t="s">
         <v>130</v>
       </c>
-      <c r="AB3" t="s">
+      <c r="AN3" t="s">
         <v>131</v>
       </c>
-      <c r="AC3" t="s">
+      <c r="AO3" t="s">
+        <v>127</v>
+      </c>
+      <c r="AP3" t="s">
         <v>132</v>
       </c>
-      <c r="AD3" t="s">
-        <v>126</v>
-      </c>
-      <c r="AE3" t="s">
-        <v>145</v>
-      </c>
-      <c r="AF3" t="s">
-        <v>146</v>
-      </c>
-      <c r="AG3" t="s">
-        <v>147</v>
-      </c>
-      <c r="AH3" t="s">
-        <v>148</v>
-      </c>
-      <c r="AI3" t="s">
-        <v>137</v>
-      </c>
-      <c r="AJ3" t="s">
-        <v>138</v>
-      </c>
-      <c r="AK3" t="s">
-        <v>149</v>
-      </c>
-      <c r="AL3" t="s">
-        <v>150</v>
-      </c>
-      <c r="AM3" t="s">
-        <v>151</v>
-      </c>
-      <c r="AN3" t="s">
-        <v>152</v>
-      </c>
-      <c r="AO3" t="s">
-        <v>138</v>
-      </c>
-      <c r="AP3" t="s">
-        <v>153</v>
-      </c>
       <c r="AQ3" t="s">
-        <v>154</v>
+        <v>133</v>
       </c>
       <c r="AR3" t="s">
-        <v>155</v>
+        <v>134</v>
       </c>
       <c r="AS3" t="s">
-        <v>156</v>
+        <v>135</v>
       </c>
       <c r="AT3" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
     </row>
     <row r="4" spans="1:46" x14ac:dyDescent="0.3">
@@ -4544,139 +4470,139 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>105</v>
+        <v>9</v>
       </c>
       <c r="C4" t="s">
         <v>106</v>
       </c>
       <c r="D4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" t="s">
         <v>107</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" t="s">
+        <v>42</v>
+      </c>
+      <c r="H4" t="s">
         <v>108</v>
       </c>
-      <c r="F4" t="s">
+      <c r="I4" t="s">
         <v>109</v>
       </c>
-      <c r="G4" t="s">
+      <c r="J4" t="s">
+        <v>13</v>
+      </c>
+      <c r="K4" t="s">
         <v>110</v>
       </c>
-      <c r="H4" t="s">
+      <c r="L4" t="s">
         <v>111</v>
       </c>
-      <c r="I4" t="s">
+      <c r="M4" t="s">
         <v>112</v>
       </c>
-      <c r="J4" t="s">
+      <c r="N4" t="s">
         <v>113</v>
       </c>
-      <c r="K4" t="s">
+      <c r="O4" t="s">
         <v>114</v>
       </c>
-      <c r="L4" t="s">
+      <c r="P4" t="s">
         <v>115</v>
       </c>
-      <c r="M4" t="s">
+      <c r="Q4" t="s">
         <v>116</v>
       </c>
-      <c r="N4" t="s">
+      <c r="R4" t="s">
         <v>117</v>
       </c>
-      <c r="O4" t="s">
+      <c r="S4" t="s">
+        <v>8</v>
+      </c>
+      <c r="T4" t="s">
         <v>118</v>
       </c>
-      <c r="P4" t="s">
+      <c r="U4" t="s">
+        <v>14</v>
+      </c>
+      <c r="V4" t="s">
         <v>119</v>
       </c>
-      <c r="Q4" t="s">
+      <c r="W4" t="s">
         <v>120</v>
       </c>
-      <c r="R4" t="s">
+      <c r="X4" t="s">
         <v>121</v>
       </c>
-      <c r="S4" t="s">
+      <c r="Y4" t="s">
+        <v>45</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>61</v>
+      </c>
+      <c r="AA4" t="s">
+        <v>136</v>
+      </c>
+      <c r="AB4" t="s">
+        <v>29</v>
+      </c>
+      <c r="AC4" t="s">
+        <v>30</v>
+      </c>
+      <c r="AD4" t="s">
         <v>122</v>
       </c>
-      <c r="T4" t="s">
-        <v>123</v>
-      </c>
-      <c r="U4" t="s">
-        <v>124</v>
-      </c>
-      <c r="V4" t="s">
-        <v>125</v>
-      </c>
-      <c r="W4" t="s">
-        <v>126</v>
-      </c>
-      <c r="X4" t="s">
+      <c r="AE4" t="s">
+        <v>120</v>
+      </c>
+      <c r="AF4" t="s">
+        <v>44</v>
+      </c>
+      <c r="AG4" t="s">
+        <v>51</v>
+      </c>
+      <c r="AH4" t="s">
+        <v>63</v>
+      </c>
+      <c r="AI4" t="s">
+        <v>137</v>
+      </c>
+      <c r="AJ4" t="s">
+        <v>35</v>
+      </c>
+      <c r="AK4" t="s">
         <v>127</v>
       </c>
-      <c r="Y4" t="s">
-        <v>157</v>
-      </c>
-      <c r="Z4" t="s">
-        <v>158</v>
-      </c>
-      <c r="AA4" t="s">
-        <v>159</v>
-      </c>
-      <c r="AB4" t="s">
-        <v>130</v>
-      </c>
-      <c r="AC4" t="s">
-        <v>131</v>
-      </c>
-      <c r="AD4" t="s">
-        <v>132</v>
-      </c>
-      <c r="AE4" t="s">
-        <v>126</v>
-      </c>
-      <c r="AF4" t="s">
-        <v>160</v>
-      </c>
-      <c r="AG4" t="s">
-        <v>161</v>
-      </c>
-      <c r="AH4" t="s">
-        <v>162</v>
-      </c>
-      <c r="AI4" t="s">
-        <v>163</v>
-      </c>
-      <c r="AJ4" t="s">
+      <c r="AL4" t="s">
+        <v>62</v>
+      </c>
+      <c r="AM4" t="s">
+        <v>138</v>
+      </c>
+      <c r="AN4" t="s">
+        <v>139</v>
+      </c>
+      <c r="AO4" t="s">
+        <v>127</v>
+      </c>
+      <c r="AP4" t="s">
+        <v>140</v>
+      </c>
+      <c r="AQ4" t="s">
         <v>137</v>
       </c>
-      <c r="AK4" t="s">
-        <v>138</v>
-      </c>
-      <c r="AL4" t="s">
-        <v>164</v>
-      </c>
-      <c r="AM4" t="s">
-        <v>165</v>
-      </c>
-      <c r="AN4" t="s">
-        <v>166</v>
-      </c>
-      <c r="AO4" t="s">
-        <v>138</v>
-      </c>
-      <c r="AP4" t="s">
-        <v>167</v>
-      </c>
-      <c r="AQ4" t="s">
-        <v>163</v>
-      </c>
       <c r="AR4" t="s">
-        <v>163</v>
+        <v>137</v>
       </c>
       <c r="AS4" t="s">
-        <v>168</v>
+        <v>70</v>
       </c>
       <c r="AT4" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
     </row>
     <row r="5" spans="1:46" x14ac:dyDescent="0.3">
@@ -4684,130 +4610,130 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>105</v>
+        <v>9</v>
       </c>
       <c r="C5" t="s">
         <v>106</v>
       </c>
       <c r="D5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" t="s">
         <v>107</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" t="s">
+        <v>42</v>
+      </c>
+      <c r="H5" t="s">
         <v>108</v>
       </c>
-      <c r="F5" t="s">
+      <c r="I5" t="s">
         <v>109</v>
       </c>
-      <c r="G5" t="s">
+      <c r="J5" t="s">
+        <v>13</v>
+      </c>
+      <c r="K5" t="s">
         <v>110</v>
       </c>
-      <c r="H5" t="s">
+      <c r="L5" t="s">
         <v>111</v>
       </c>
-      <c r="I5" t="s">
+      <c r="M5" t="s">
         <v>112</v>
       </c>
-      <c r="J5" t="s">
+      <c r="N5" t="s">
         <v>113</v>
       </c>
-      <c r="K5" t="s">
+      <c r="O5" t="s">
         <v>114</v>
       </c>
-      <c r="L5" t="s">
+      <c r="P5" t="s">
         <v>115</v>
       </c>
-      <c r="M5" t="s">
+      <c r="Q5" t="s">
         <v>116</v>
       </c>
-      <c r="N5" t="s">
+      <c r="R5" t="s">
         <v>117</v>
       </c>
-      <c r="O5" t="s">
+      <c r="S5" t="s">
+        <v>8</v>
+      </c>
+      <c r="T5" t="s">
         <v>118</v>
       </c>
-      <c r="P5" t="s">
+      <c r="U5" t="s">
+        <v>14</v>
+      </c>
+      <c r="V5" t="s">
         <v>119</v>
       </c>
-      <c r="Q5" t="s">
+      <c r="W5" t="s">
         <v>120</v>
       </c>
-      <c r="R5" t="s">
+      <c r="X5" t="s">
         <v>121</v>
       </c>
-      <c r="S5" t="s">
+      <c r="Y5" t="s">
+        <v>33</v>
+      </c>
+      <c r="Z5" t="s">
+        <v>26</v>
+      </c>
+      <c r="AA5" t="s">
+        <v>29</v>
+      </c>
+      <c r="AB5" t="s">
+        <v>30</v>
+      </c>
+      <c r="AC5" t="s">
         <v>122</v>
       </c>
-      <c r="T5" t="s">
-        <v>123</v>
-      </c>
-      <c r="U5" t="s">
-        <v>124</v>
-      </c>
-      <c r="V5" t="s">
-        <v>125</v>
-      </c>
-      <c r="W5" t="s">
-        <v>126</v>
-      </c>
-      <c r="X5" t="s">
+      <c r="AD5" t="s">
+        <v>120</v>
+      </c>
+      <c r="AE5" t="s">
+        <v>141</v>
+      </c>
+      <c r="AF5" t="s">
+        <v>142</v>
+      </c>
+      <c r="AG5" t="s">
+        <v>143</v>
+      </c>
+      <c r="AH5" t="s">
+        <v>143</v>
+      </c>
+      <c r="AI5" t="s">
+        <v>35</v>
+      </c>
+      <c r="AJ5" t="s">
         <v>127</v>
       </c>
-      <c r="Y5" t="s">
-        <v>169</v>
-      </c>
-      <c r="Z5" t="s">
-        <v>128</v>
-      </c>
-      <c r="AA5" t="s">
-        <v>130</v>
-      </c>
-      <c r="AB5" t="s">
-        <v>131</v>
-      </c>
-      <c r="AC5" t="s">
-        <v>132</v>
-      </c>
-      <c r="AD5" t="s">
-        <v>126</v>
-      </c>
-      <c r="AE5" t="s">
-        <v>133</v>
-      </c>
-      <c r="AF5" t="s">
-        <v>135</v>
-      </c>
-      <c r="AG5" t="s">
-        <v>170</v>
-      </c>
-      <c r="AH5" t="s">
-        <v>170</v>
-      </c>
-      <c r="AI5" t="s">
-        <v>137</v>
-      </c>
-      <c r="AJ5" t="s">
-        <v>138</v>
-      </c>
       <c r="AK5" t="s">
-        <v>170</v>
+        <v>143</v>
       </c>
       <c r="AL5" t="s">
-        <v>170</v>
+        <v>143</v>
       </c>
       <c r="AM5" t="s">
-        <v>170</v>
+        <v>143</v>
       </c>
       <c r="AN5" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="AO5" t="s">
-        <v>138</v>
+        <v>127</v>
       </c>
       <c r="AP5" t="s">
-        <v>138</v>
+        <v>127</v>
       </c>
       <c r="AQ5" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
     </row>
     <row r="6" spans="1:46" x14ac:dyDescent="0.3">
@@ -4815,130 +4741,130 @@
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>105</v>
+        <v>9</v>
       </c>
       <c r="C6" t="s">
         <v>106</v>
       </c>
       <c r="D6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" t="s">
         <v>107</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6" t="s">
+        <v>42</v>
+      </c>
+      <c r="H6" t="s">
         <v>108</v>
       </c>
-      <c r="F6" t="s">
+      <c r="I6" t="s">
         <v>109</v>
       </c>
-      <c r="G6" t="s">
+      <c r="J6" t="s">
+        <v>13</v>
+      </c>
+      <c r="K6" t="s">
         <v>110</v>
       </c>
-      <c r="H6" t="s">
+      <c r="L6" t="s">
         <v>111</v>
       </c>
-      <c r="I6" t="s">
+      <c r="M6" t="s">
         <v>112</v>
       </c>
-      <c r="J6" t="s">
+      <c r="N6" t="s">
         <v>113</v>
       </c>
-      <c r="K6" t="s">
+      <c r="O6" t="s">
         <v>114</v>
       </c>
-      <c r="L6" t="s">
+      <c r="P6" t="s">
         <v>115</v>
       </c>
-      <c r="M6" t="s">
+      <c r="Q6" t="s">
         <v>116</v>
       </c>
-      <c r="N6" t="s">
+      <c r="R6" t="s">
         <v>117</v>
       </c>
-      <c r="O6" t="s">
+      <c r="S6" t="s">
+        <v>8</v>
+      </c>
+      <c r="T6" t="s">
         <v>118</v>
       </c>
-      <c r="P6" t="s">
+      <c r="U6" t="s">
+        <v>14</v>
+      </c>
+      <c r="V6" t="s">
         <v>119</v>
       </c>
-      <c r="Q6" t="s">
+      <c r="W6" t="s">
+        <v>105</v>
+      </c>
+      <c r="X6" t="s">
+        <v>121</v>
+      </c>
+      <c r="Y6" t="s">
+        <v>145</v>
+      </c>
+      <c r="Z6" t="s">
+        <v>73</v>
+      </c>
+      <c r="AA6" t="s">
+        <v>146</v>
+      </c>
+      <c r="AB6" t="s">
+        <v>29</v>
+      </c>
+      <c r="AC6" t="s">
+        <v>30</v>
+      </c>
+      <c r="AD6" t="s">
+        <v>122</v>
+      </c>
+      <c r="AE6" t="s">
         <v>120</v>
       </c>
-      <c r="R6" t="s">
-        <v>121</v>
-      </c>
-      <c r="S6" t="s">
-        <v>122</v>
-      </c>
-      <c r="T6" t="s">
-        <v>123</v>
-      </c>
-      <c r="U6" t="s">
-        <v>124</v>
-      </c>
-      <c r="V6" t="s">
-        <v>125</v>
-      </c>
-      <c r="W6" t="s">
-        <v>171</v>
-      </c>
-      <c r="X6" t="s">
+      <c r="AF6" t="s">
+        <v>141</v>
+      </c>
+      <c r="AG6" t="s">
+        <v>147</v>
+      </c>
+      <c r="AH6" t="s">
+        <v>148</v>
+      </c>
+      <c r="AI6" t="s">
+        <v>35</v>
+      </c>
+      <c r="AJ6" t="s">
         <v>127</v>
       </c>
-      <c r="Y6" t="s">
-        <v>129</v>
-      </c>
-      <c r="Z6" t="s">
-        <v>172</v>
-      </c>
-      <c r="AA6" t="s">
-        <v>173</v>
-      </c>
-      <c r="AB6" t="s">
-        <v>130</v>
-      </c>
-      <c r="AC6" t="s">
-        <v>131</v>
-      </c>
-      <c r="AD6" t="s">
-        <v>132</v>
-      </c>
-      <c r="AE6" t="s">
-        <v>126</v>
-      </c>
-      <c r="AF6" t="s">
-        <v>133</v>
-      </c>
-      <c r="AG6" t="s">
-        <v>174</v>
-      </c>
-      <c r="AH6" t="s">
-        <v>134</v>
-      </c>
-      <c r="AI6" t="s">
-        <v>137</v>
-      </c>
-      <c r="AJ6" t="s">
-        <v>138</v>
-      </c>
       <c r="AK6" t="s">
-        <v>175</v>
+        <v>149</v>
       </c>
       <c r="AL6" t="s">
-        <v>176</v>
+        <v>150</v>
       </c>
       <c r="AM6" t="s">
-        <v>177</v>
+        <v>151</v>
       </c>
       <c r="AN6" t="s">
-        <v>178</v>
+        <v>83</v>
       </c>
       <c r="AO6" t="s">
-        <v>138</v>
+        <v>127</v>
       </c>
       <c r="AP6" t="s">
-        <v>179</v>
+        <v>152</v>
       </c>
       <c r="AQ6" s="1" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
     </row>
     <row r="7" spans="1:46" x14ac:dyDescent="0.3">
@@ -4946,130 +4872,130 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>105</v>
+        <v>9</v>
       </c>
       <c r="C7" t="s">
         <v>106</v>
       </c>
       <c r="D7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" t="s">
         <v>107</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7" t="s">
+        <v>42</v>
+      </c>
+      <c r="H7" t="s">
         <v>108</v>
       </c>
-      <c r="F7" t="s">
+      <c r="I7" t="s">
         <v>109</v>
       </c>
-      <c r="G7" t="s">
+      <c r="J7" t="s">
+        <v>13</v>
+      </c>
+      <c r="K7" t="s">
         <v>110</v>
       </c>
-      <c r="H7" t="s">
+      <c r="L7" t="s">
         <v>111</v>
       </c>
-      <c r="I7" t="s">
+      <c r="M7" t="s">
         <v>112</v>
       </c>
-      <c r="J7" t="s">
+      <c r="N7" t="s">
         <v>113</v>
       </c>
-      <c r="K7" t="s">
+      <c r="O7" t="s">
         <v>114</v>
       </c>
-      <c r="L7" t="s">
+      <c r="P7" t="s">
         <v>115</v>
       </c>
-      <c r="M7" t="s">
+      <c r="Q7" t="s">
         <v>116</v>
       </c>
-      <c r="N7" t="s">
+      <c r="R7" t="s">
         <v>117</v>
       </c>
-      <c r="O7" t="s">
+      <c r="S7" t="s">
+        <v>8</v>
+      </c>
+      <c r="T7" t="s">
         <v>118</v>
       </c>
-      <c r="P7" t="s">
+      <c r="U7" t="s">
+        <v>14</v>
+      </c>
+      <c r="V7" t="s">
         <v>119</v>
       </c>
-      <c r="Q7" t="s">
+      <c r="W7" t="s">
+        <v>121</v>
+      </c>
+      <c r="X7" t="s">
+        <v>153</v>
+      </c>
+      <c r="Y7" t="s">
+        <v>154</v>
+      </c>
+      <c r="Z7" t="s">
+        <v>155</v>
+      </c>
+      <c r="AA7" t="s">
+        <v>29</v>
+      </c>
+      <c r="AB7" t="s">
+        <v>30</v>
+      </c>
+      <c r="AC7" t="s">
+        <v>122</v>
+      </c>
+      <c r="AD7" t="s">
+        <v>156</v>
+      </c>
+      <c r="AE7" t="s">
+        <v>157</v>
+      </c>
+      <c r="AF7" t="s">
+        <v>158</v>
+      </c>
+      <c r="AG7" t="s">
+        <v>159</v>
+      </c>
+      <c r="AH7" t="s">
+        <v>35</v>
+      </c>
+      <c r="AI7" t="s">
+        <v>127</v>
+      </c>
+      <c r="AJ7" t="s">
         <v>120</v>
       </c>
-      <c r="R7" t="s">
-        <v>121</v>
-      </c>
-      <c r="S7" t="s">
-        <v>122</v>
-      </c>
-      <c r="T7" t="s">
-        <v>123</v>
-      </c>
-      <c r="U7" t="s">
-        <v>124</v>
-      </c>
-      <c r="V7" t="s">
-        <v>125</v>
-      </c>
-      <c r="W7" t="s">
+      <c r="AK7" t="s">
+        <v>100</v>
+      </c>
+      <c r="AL7" t="s">
+        <v>160</v>
+      </c>
+      <c r="AM7" t="s">
         <v>127</v>
       </c>
-      <c r="X7" t="s">
-        <v>180</v>
-      </c>
-      <c r="Y7" t="s">
-        <v>181</v>
-      </c>
-      <c r="Z7" t="s">
-        <v>182</v>
-      </c>
-      <c r="AA7" t="s">
-        <v>130</v>
-      </c>
-      <c r="AB7" t="s">
-        <v>131</v>
-      </c>
-      <c r="AC7" t="s">
-        <v>132</v>
-      </c>
-      <c r="AD7" t="s">
-        <v>183</v>
-      </c>
-      <c r="AE7" t="s">
-        <v>184</v>
-      </c>
-      <c r="AF7" t="s">
-        <v>185</v>
-      </c>
-      <c r="AG7" t="s">
-        <v>186</v>
-      </c>
-      <c r="AH7" t="s">
-        <v>137</v>
-      </c>
-      <c r="AI7" t="s">
-        <v>138</v>
-      </c>
-      <c r="AJ7" t="s">
-        <v>126</v>
-      </c>
-      <c r="AK7" t="s">
-        <v>187</v>
-      </c>
-      <c r="AL7" t="s">
-        <v>188</v>
-      </c>
-      <c r="AM7" t="s">
-        <v>138</v>
-      </c>
       <c r="AN7" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="AO7" t="s">
-        <v>189</v>
+        <v>102</v>
       </c>
       <c r="AP7" t="s">
-        <v>190</v>
+        <v>161</v>
       </c>
       <c r="AQ7" s="1" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
     </row>
     <row r="8" spans="1:46" x14ac:dyDescent="0.3">
@@ -5077,127 +5003,128 @@
         <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>105</v>
+        <v>9</v>
       </c>
       <c r="C8" t="s">
         <v>106</v>
       </c>
       <c r="D8" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" t="s">
         <v>107</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
+        <v>10</v>
+      </c>
+      <c r="G8" t="s">
+        <v>42</v>
+      </c>
+      <c r="H8" t="s">
         <v>108</v>
       </c>
-      <c r="F8" t="s">
+      <c r="I8" t="s">
         <v>109</v>
       </c>
-      <c r="G8" t="s">
+      <c r="J8" t="s">
+        <v>13</v>
+      </c>
+      <c r="K8" t="s">
         <v>110</v>
       </c>
-      <c r="H8" t="s">
+      <c r="L8" t="s">
         <v>111</v>
       </c>
-      <c r="I8" t="s">
+      <c r="M8" t="s">
         <v>112</v>
       </c>
-      <c r="J8" t="s">
+      <c r="N8" t="s">
         <v>113</v>
       </c>
-      <c r="K8" t="s">
+      <c r="O8" t="s">
         <v>114</v>
       </c>
-      <c r="L8" t="s">
+      <c r="P8" t="s">
         <v>115</v>
       </c>
-      <c r="M8" t="s">
+      <c r="Q8" t="s">
         <v>116</v>
       </c>
-      <c r="N8" t="s">
+      <c r="R8" t="s">
         <v>117</v>
       </c>
-      <c r="O8" t="s">
+      <c r="S8" t="s">
+        <v>8</v>
+      </c>
+      <c r="T8" t="s">
         <v>118</v>
       </c>
-      <c r="P8" t="s">
+      <c r="U8" t="s">
+        <v>14</v>
+      </c>
+      <c r="V8" t="s">
         <v>119</v>
       </c>
-      <c r="Q8" t="s">
+      <c r="W8" t="s">
         <v>120</v>
       </c>
-      <c r="R8" t="s">
+      <c r="X8" t="s">
         <v>121</v>
       </c>
-      <c r="S8" t="s">
+      <c r="Y8" t="s">
+        <v>162</v>
+      </c>
+      <c r="Z8" t="s">
+        <v>29</v>
+      </c>
+      <c r="AA8" t="s">
+        <v>30</v>
+      </c>
+      <c r="AB8" t="s">
         <v>122</v>
       </c>
-      <c r="T8" t="s">
-        <v>123</v>
-      </c>
-      <c r="U8" t="s">
-        <v>124</v>
-      </c>
-      <c r="V8" t="s">
-        <v>125</v>
-      </c>
-      <c r="W8" t="s">
-        <v>126</v>
-      </c>
-      <c r="X8" t="s">
+      <c r="AC8" t="s">
+        <v>120</v>
+      </c>
+      <c r="AD8" t="s">
+        <v>45</v>
+      </c>
+      <c r="AE8" t="s">
+        <v>163</v>
+      </c>
+      <c r="AF8" t="s">
+        <v>164</v>
+      </c>
+      <c r="AG8" t="s">
+        <v>165</v>
+      </c>
+      <c r="AH8" t="s">
+        <v>35</v>
+      </c>
+      <c r="AI8" t="s">
         <v>127</v>
       </c>
-      <c r="Y8" t="s">
-        <v>191</v>
-      </c>
-      <c r="Z8" t="s">
-        <v>130</v>
-      </c>
-      <c r="AA8" t="s">
-        <v>131</v>
-      </c>
-      <c r="AB8" t="s">
-        <v>132</v>
-      </c>
-      <c r="AC8" t="s">
-        <v>126</v>
-      </c>
-      <c r="AD8" t="s">
-        <v>157</v>
-      </c>
-      <c r="AE8" t="s">
-        <v>192</v>
-      </c>
-      <c r="AF8" t="s">
-        <v>193</v>
-      </c>
-      <c r="AG8" t="s">
-        <v>194</v>
-      </c>
-      <c r="AH8" t="s">
-        <v>137</v>
-      </c>
-      <c r="AI8" t="s">
-        <v>138</v>
-      </c>
       <c r="AJ8" t="s">
-        <v>134</v>
+        <v>148</v>
       </c>
       <c r="AK8" t="s">
-        <v>195</v>
+        <v>166</v>
       </c>
       <c r="AL8" t="s">
-        <v>196</v>
+        <v>167</v>
       </c>
       <c r="AM8" t="s">
-        <v>197</v>
+        <v>168</v>
       </c>
       <c r="AN8" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="AO8" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>